<commit_message>
Several rows supplemented in the three RDA files containing ChartSettings.
</commit_message>
<xml_diff>
--- a/Input/Excel/Parameters_ExpectationRanges.xlsx
+++ b/Input/Excel/Parameters_ExpectationRanges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TL\Entwicklung\R\GitHub\myRepos\TabulaCharts\Input\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2860288D-3EE2-465D-A687-5C637ABF5431}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719CE2FF-7262-454D-80D4-348F1F75A1C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12168" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13104" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChartData" sheetId="5" r:id="rId1"/>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="163">
   <si>
     <t>VarName</t>
   </si>
@@ -779,9 +779,6 @@
     <t>Final Energy DHW</t>
   </si>
   <si>
-    <t>ExpectationRange.01</t>
-  </si>
-  <si>
     <t>Erwartungsbereiche</t>
   </si>
   <si>
@@ -1020,6 +1017,18 @@
   </si>
   <si>
     <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>ExpectationRanges.01</t>
+  </si>
+  <si>
+    <t>ExpectationRanges.02</t>
+  </si>
+  <si>
+    <t>ExpectationRanges.03</t>
+  </si>
+  <si>
+    <t>ExpectationRanges.04</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1088,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1118,6 +1127,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1470,7 +1482,7 @@
         <v>55</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
@@ -1488,10 +1500,10 @@
         <v>55</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>34</v>
@@ -1502,10 +1514,10 @@
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -1523,10 +1535,10 @@
         <v>55</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>34</v>
@@ -1537,16 +1549,16 @@
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>58</v>
@@ -1558,10 +1570,10 @@
         <v>55</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>34</v>
@@ -1572,16 +1584,16 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>58</v>
@@ -1593,10 +1605,10 @@
         <v>55</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>34</v>
@@ -1610,7 +1622,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
@@ -1628,10 +1640,10 @@
         <v>52</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>3</v>
@@ -1642,10 +1654,10 @@
     </row>
     <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -1663,10 +1675,10 @@
         <v>52</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>3</v>
@@ -1677,16 +1689,16 @@
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>59</v>
@@ -1698,10 +1710,10 @@
         <v>52</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>3</v>
@@ -1712,16 +1724,16 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>59</v>
@@ -1733,10 +1745,10 @@
         <v>52</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>3</v>
@@ -1750,7 +1762,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
@@ -1768,10 +1780,10 @@
         <v>54</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>33</v>
@@ -1782,10 +1794,10 @@
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1803,10 +1815,10 @@
         <v>54</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>33</v>
@@ -1817,16 +1829,16 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>60</v>
@@ -1838,10 +1850,10 @@
         <v>54</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>33</v>
@@ -1852,16 +1864,16 @@
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="3">
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>60</v>
@@ -1873,10 +1885,10 @@
         <v>54</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>33</v>
@@ -1890,7 +1902,7 @@
         <v>66</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -1908,10 +1920,10 @@
         <v>66</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>36</v>
@@ -1922,10 +1934,10 @@
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -1943,10 +1955,10 @@
         <v>66</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>36</v>
@@ -1957,16 +1969,16 @@
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>76</v>
@@ -1978,10 +1990,10 @@
         <v>66</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>36</v>
@@ -1992,10 +2004,10 @@
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -2013,10 +2025,10 @@
         <v>66</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>36</v>
@@ -2030,7 +2042,7 @@
         <v>64</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="8">
         <v>2</v>
@@ -2048,10 +2060,10 @@
         <v>64</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>35</v>
@@ -2062,10 +2074,10 @@
     </row>
     <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
@@ -2083,10 +2095,10 @@
         <v>64</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>35</v>
@@ -2097,16 +2109,16 @@
     </row>
     <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>75</v>
@@ -2118,10 +2130,10 @@
         <v>64</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>35</v>
@@ -2132,10 +2144,10 @@
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
@@ -2153,10 +2165,10 @@
         <v>64</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>35</v>
@@ -2170,7 +2182,7 @@
         <v>65</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="8">
         <v>3</v>
@@ -2188,10 +2200,10 @@
         <v>65</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>37</v>
@@ -2202,10 +2214,10 @@
     </row>
     <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="C23" s="6">
         <v>3</v>
@@ -2223,10 +2235,10 @@
         <v>65</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>37</v>
@@ -2237,16 +2249,16 @@
     </row>
     <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" s="3">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>71</v>
@@ -2258,10 +2270,10 @@
         <v>65</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>37</v>
@@ -2272,10 +2284,10 @@
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25" s="3">
         <v>3</v>
@@ -2293,10 +2305,10 @@
         <v>65</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>37</v>
@@ -2310,7 +2322,7 @@
         <v>62</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -2328,10 +2340,10 @@
         <v>62</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>39</v>
@@ -2342,10 +2354,10 @@
     </row>
     <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
@@ -2363,10 +2375,10 @@
         <v>62</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>39</v>
@@ -2377,16 +2389,16 @@
     </row>
     <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>78</v>
@@ -2398,10 +2410,10 @@
         <v>62</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>39</v>
@@ -2412,10 +2424,10 @@
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -2433,10 +2445,10 @@
         <v>62</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>39</v>
@@ -2450,7 +2462,7 @@
         <v>61</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
@@ -2468,10 +2480,10 @@
         <v>61</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>38</v>
@@ -2482,10 +2494,10 @@
     </row>
     <row r="31" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
@@ -2503,10 +2515,10 @@
         <v>61</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>38</v>
@@ -2517,16 +2529,16 @@
     </row>
     <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3">
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>77</v>
@@ -2538,10 +2550,10 @@
         <v>61</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>38</v>
@@ -2552,10 +2564,10 @@
     </row>
     <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" s="3">
         <v>2</v>
@@ -2573,10 +2585,10 @@
         <v>61</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>38</v>
@@ -2590,7 +2602,7 @@
         <v>63</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C34" s="8">
         <v>3</v>
@@ -2608,10 +2620,10 @@
         <v>63</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>51</v>
@@ -2622,10 +2634,10 @@
     </row>
     <row r="35" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="6">
         <v>3</v>
@@ -2643,10 +2655,10 @@
         <v>63</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>51</v>
@@ -2657,16 +2669,16 @@
     </row>
     <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>70</v>
@@ -2678,10 +2690,10 @@
         <v>63</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>51</v>
@@ -2692,10 +2704,10 @@
     </row>
     <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
@@ -2713,10 +2725,10 @@
         <v>63</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>51</v>
@@ -2733,13 +2745,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999E11F1-4A6B-4F19-9DE9-82D2F58C1417}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2838,25 +2850,28 @@
     </row>
     <row r="2" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="13">
+        <v>45541</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
         <v>81</v>
       </c>
-      <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
         <v>83</v>
       </c>
-      <c r="H2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>84</v>
-      </c>
-      <c r="P2" t="s">
-        <v>85</v>
       </c>
       <c r="R2">
         <v>20</v>
@@ -2868,7 +2883,7 @@
         <v>0.12</v>
       </c>
       <c r="U2" s="2">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="V2" s="2">
         <v>0.3</v>
@@ -2889,6 +2904,183 @@
         <v>5</v>
       </c>
       <c r="AB2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="13">
+        <v>45478</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>400</v>
+      </c>
+      <c r="Z3">
+        <v>20</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
+      </c>
+      <c r="AB3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="13">
+        <v>45541</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" t="s">
+        <v>84</v>
+      </c>
+      <c r="R4">
+        <v>20</v>
+      </c>
+      <c r="S4">
+        <v>20</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>400</v>
+      </c>
+      <c r="Z4">
+        <v>20</v>
+      </c>
+      <c r="AA4">
+        <v>5</v>
+      </c>
+      <c r="AB4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="13">
+        <v>45541</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" t="s">
+        <v>84</v>
+      </c>
+      <c r="R5">
+        <v>20</v>
+      </c>
+      <c r="S5">
+        <v>20</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>400</v>
+      </c>
+      <c r="Z5">
+        <v>20</v>
+      </c>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A new function has been added for comparing values from different datasets.
</commit_message>
<xml_diff>
--- a/Input/Excel/Parameters_ExpectationRanges.xlsx
+++ b/Input/Excel/Parameters_ExpectationRanges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TL\Entwicklung\R\GitHub\myRepos\TabulaCharts\Input\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TL\Entwicklung\R\GitHub\myRepos\TabulaCharts\Input\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719CE2FF-7262-454D-80D4-348F1F75A1C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A4F59-857F-4AD4-8ADA-6789B35B9115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13104" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13104" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChartData" sheetId="5" r:id="rId1"/>
@@ -59,6 +59,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{8B5FEC8D-1AB1-44E5-9B4F-274641673899}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D2965E57-523F-40B7-8A2D-3E06F56B9A8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J3" authorId="0" shapeId="0" xr:uid="{F2BB52A0-6B8A-4415-A09D-5BF00C178D40}">
       <text>
         <r>
@@ -87,6 +115,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{4BA765A9-5BAB-49DA-8A1D-B8614E72D1AA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{9E61121F-6424-4057-B12A-74FA37292F52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J6" authorId="0" shapeId="0" xr:uid="{882EE04A-5099-4629-84F7-F8B5F1E2A3B9}">
       <text>
         <r>
@@ -115,6 +171,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{AEB10DAA-190B-4DBE-8859-C04E0FAECDB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{871CF341-AD96-4C5B-AF33-6E2A29756124}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J7" authorId="0" shapeId="0" xr:uid="{6C55CC23-1161-4182-8A9F-AFE5663ADB93}">
       <text>
         <r>
@@ -143,6 +227,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{51DE6C23-4041-4A17-BE05-654178F08F11}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{C381D886-168C-456E-9BD3-A484D99CB292}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J10" authorId="0" shapeId="0" xr:uid="{9E2194C8-6B3B-4F60-914F-096BFDC8B006}">
       <text>
         <r>
@@ -171,6 +283,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{B3DF08C0-26CE-4634-83DF-270DDE6D499F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{8E18FC3D-48AA-453B-BAAC-2F558D965181}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 blank = Heat need</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J11" authorId="0" shapeId="0" xr:uid="{F48DCDD2-73A9-4CEA-A1FB-5746E886DFA8}">
       <text>
         <r>
@@ -199,6 +339,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{AA657E58-407E-4909-9CF0-85D03A7A8719}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{8A411CB6-DEC0-4C24-9847-DD1D2E28B316}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>4 blanks = Heat need minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J14" authorId="0" shapeId="0" xr:uid="{B71E50C0-0FF9-4C4E-AB94-1A48CEA44AB2}">
       <text>
         <r>
@@ -227,6 +395,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{F837223A-0E53-49B2-9AE8-682655D60EDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N14" authorId="0" shapeId="0" xr:uid="{EED97F72-D51A-47D6-A90D-BE515DF8CE15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J15" authorId="0" shapeId="0" xr:uid="{B50AE5F3-7473-4986-891C-33BE2D696FA4}">
       <text>
         <r>
@@ -255,6 +451,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M15" authorId="0" shapeId="0" xr:uid="{28693E79-DE69-4C06-823C-109C2EC8E143}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N15" authorId="0" shapeId="0" xr:uid="{62D5A4C3-4BA2-407A-977E-67E208494AF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J18" authorId="0" shapeId="0" xr:uid="{AD51558F-7583-4720-AC21-707E5367ECD6}">
       <text>
         <r>
@@ -283,6 +507,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M18" authorId="0" shapeId="0" xr:uid="{A6964922-53C0-4B0A-BF72-CFC155615C6C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N18" authorId="0" shapeId="0" xr:uid="{ADBB8E5F-EDB7-4E0B-9FA3-547BE251696B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J19" authorId="0" shapeId="0" xr:uid="{6047E77B-1D98-4AF5-B5A6-E79FBAB2404D}">
       <text>
         <r>
@@ -311,6 +563,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{247705E0-E486-4A07-AD57-CB14A8FF3CC1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N19" authorId="0" shapeId="0" xr:uid="{DC22C64A-AE76-420F-B489-B1A395D53D7E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J22" authorId="0" shapeId="0" xr:uid="{F84FA6A8-8E4B-4265-9C87-F72AB6184A5D}">
       <text>
         <r>
@@ -339,6 +619,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{EFA76C81-9F9F-4B23-AF90-0CAAD77A0D40}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{DF74AFB3-6A1A-4E5E-9952-4D71529B386B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 blanks = Heat generation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J23" authorId="0" shapeId="0" xr:uid="{1B1852B2-5C0E-402B-9496-E5CAFB73E04A}">
       <text>
         <r>
@@ -367,6 +675,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{B35CBC39-A356-4905-A2A0-3CCC8C6DE762}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N23" authorId="0" shapeId="0" xr:uid="{F0A20582-4175-4951-8F45-26DB0B90DFD4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>5 blanks = Heat generation minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J26" authorId="0" shapeId="0" xr:uid="{E6FFD222-5929-4EFC-9243-8F1B5FC24A32}">
       <text>
         <r>
@@ -395,6 +731,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M26" authorId="0" shapeId="0" xr:uid="{8F87A0CE-A946-4FE3-81E8-1A4BC3E640D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N26" authorId="0" shapeId="0" xr:uid="{139A2AC9-4080-4CFF-AC16-A9B13673A1F3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J27" authorId="0" shapeId="0" xr:uid="{7EF53B43-2892-4411-A1A6-FA9B8BEAF7BE}">
       <text>
         <r>
@@ -423,6 +787,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{47549C93-0162-4F71-8AAD-36BE2ECD7CD2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N27" authorId="0" shapeId="0" xr:uid="{AF5B0623-57ED-4B9C-8D38-B76B3A73C59D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J30" authorId="0" shapeId="0" xr:uid="{06D1D5E6-C1E1-4856-9A02-B9E1B86DE51D}">
       <text>
         <r>
@@ -451,6 +843,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M30" authorId="0" shapeId="0" xr:uid="{26346C7F-B501-4A49-9604-94597FCD16C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N30" authorId="0" shapeId="0" xr:uid="{E7EFA0DA-DC91-4125-BE77-0000A27913C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J31" authorId="0" shapeId="0" xr:uid="{B7CAD671-B229-4E07-AF81-BA85D25E2E87}">
       <text>
         <r>
@@ -479,6 +899,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M31" authorId="0" shapeId="0" xr:uid="{B84A5EB7-6A64-4F76-B2C1-E1DBE7D64239}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N31" authorId="0" shapeId="0" xr:uid="{EDFF1568-416F-4452-9DCF-E9FDA5886C84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J34" authorId="0" shapeId="0" xr:uid="{A97C86C4-449D-4468-9900-04367E1A9EF3}">
       <text>
         <r>
@@ -507,6 +955,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="M34" authorId="0" shapeId="0" xr:uid="{AAAA499C-71D0-47B2-9400-A1414EDD47DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N34" authorId="0" shapeId="0" xr:uid="{52C500C1-D993-4325-AE68-66F685B8CC96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>3 blanks = Final energy</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J35" authorId="0" shapeId="0" xr:uid="{478FC361-EF48-480F-9EDA-05D22D4073A5}">
       <text>
         <r>
@@ -522,6 +998,34 @@
       </text>
     </comment>
     <comment ref="K35" authorId="0" shapeId="0" xr:uid="{7A1C8749-E184-4E41-B26C-3BD380134B89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M35" authorId="0" shapeId="0" xr:uid="{6CF73E01-81CC-44E2-8EC2-C9BC0B418181}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 blanks = Final energy minus StdDev</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N35" authorId="0" shapeId="0" xr:uid="{C4D2C282-53F2-4B04-AA58-50B2EBD872C3}">
       <text>
         <r>
           <rPr>
@@ -540,7 +1044,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="178">
   <si>
     <t>VarName</t>
   </si>
@@ -713,9 +1217,6 @@
     <t>Heizwärmebedarf</t>
   </si>
   <si>
-    <t>Nutzwärmebedarf Warmwasser</t>
-  </si>
-  <si>
     <t>Usable heat need DHW</t>
   </si>
   <si>
@@ -743,27 +1244,12 @@
     <t>q_g_out_w_sum</t>
   </si>
   <si>
-    <t>Wärmeerzeugung Heizung</t>
-  </si>
-  <si>
-    <t>Wärmeerzeugung Warmwasser</t>
-  </si>
-  <si>
-    <t>Wärmeerzeugung Gesamt</t>
-  </si>
-  <si>
     <t>Final energy total</t>
   </si>
   <si>
     <t>Heat generation total</t>
   </si>
   <si>
-    <t>Endenergie Heizung</t>
-  </si>
-  <si>
-    <t>Endenergie Warmwasser</t>
-  </si>
-  <si>
     <t>Endenergie Gesamt</t>
   </si>
   <si>
@@ -1029,6 +1515,69 @@
   </si>
   <si>
     <t>ExpectationRanges.04</t>
+  </si>
+  <si>
+    <t>Label_Short_ENG</t>
+  </si>
+  <si>
+    <t>Label_Short_GER</t>
+  </si>
+  <si>
+    <t>Label_Short_XXX</t>
+  </si>
+  <si>
+    <t>Wärmebedarf unten</t>
+  </si>
+  <si>
+    <t>Wärmebedarf oben</t>
+  </si>
+  <si>
+    <t>Wärmeerzeugung unten</t>
+  </si>
+  <si>
+    <t>Wärmeerzeugung oben</t>
+  </si>
+  <si>
+    <t>Endenergie unten</t>
+  </si>
+  <si>
+    <t>Endenergie oben</t>
+  </si>
+  <si>
+    <t>Heat need lower</t>
+  </si>
+  <si>
+    <t>Heat need upper</t>
+  </si>
+  <si>
+    <t>Heat generation lower</t>
+  </si>
+  <si>
+    <t>Heat generation upper</t>
+  </si>
+  <si>
+    <t>Final energy lower</t>
+  </si>
+  <si>
+    <t>Final energy upper</t>
+  </si>
+  <si>
+    <t>Wärmeerzeugung Hzg</t>
+  </si>
+  <si>
+    <t>Endenergie Hzg</t>
+  </si>
+  <si>
+    <t>Nutzwärmebedarf WW</t>
+  </si>
+  <si>
+    <t>Wärmeerzeugung WW</t>
+  </si>
+  <si>
+    <t>Endenergie WW</t>
+  </si>
+  <si>
+    <t>Wärmeerz. Gesamt</t>
   </si>
 </sst>
 </file>
@@ -1416,13 +1965,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E45032B-2E80-4D51-B0CF-A465C8721EB5}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,11 +1981,11 @@
     <col min="3" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="8" width="26.77734375" customWidth="1"/>
     <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="12" width="31.21875" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
+    <col min="10" max="15" width="31.21875" customWidth="1"/>
+    <col min="16" max="16" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1473,16 +2022,25 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
@@ -1491,33 +2049,42 @@
         <v>#N/A</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -1526,103 +2093,130 @@
         <v>#N/A</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>55</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
@@ -1631,7 +2225,7 @@
         <v>#N/A</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>53</v>
@@ -1640,24 +2234,33 @@
         <v>52</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -1666,7 +2269,7 @@
         <v>#N/A</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>53</v>
@@ -1675,33 +2278,42 @@
         <v>52</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>53</v>
@@ -1710,33 +2322,42 @@
         <v>52</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>53</v>
@@ -1745,24 +2366,33 @@
         <v>52</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
@@ -1771,7 +2401,7 @@
         <v>#N/A</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>56</v>
@@ -1780,24 +2410,33 @@
         <v>54</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1806,7 +2445,7 @@
         <v>#N/A</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>56</v>
@@ -1815,33 +2454,42 @@
         <v>54</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>56</v>
@@ -1850,33 +2498,42 @@
         <v>54</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C13" s="3">
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>56</v>
@@ -1885,24 +2542,33 @@
         <v>54</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -1911,33 +2577,42 @@
         <v>#N/A</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -1946,68 +2621,86 @@
         <v>#N/A</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -2016,33 +2709,42 @@
         <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C18" s="8">
         <v>2</v>
@@ -2051,33 +2753,42 @@
         <v>#N/A</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
@@ -2086,68 +2797,86 @@
         <v>#N/A</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
@@ -2156,33 +2885,42 @@
         <v>14</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C22" s="8">
         <v>3</v>
@@ -2191,33 +2929,42 @@
         <v>#N/A</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C23" s="6">
         <v>3</v>
@@ -2226,68 +2973,86 @@
         <v>#N/A</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="M23" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C24" s="3">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C25" s="3">
         <v>3</v>
@@ -2296,33 +3061,42 @@
         <v>14</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -2331,33 +3105,42 @@
         <v>#N/A</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
@@ -2366,68 +3149,86 @@
         <v>#N/A</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M27" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -2436,33 +3237,42 @@
         <v>13</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
@@ -2471,33 +3281,42 @@
         <v>#N/A</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M30" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
@@ -2506,68 +3325,86 @@
         <v>#N/A</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M31" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M31" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P31" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C32" s="3">
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M32" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C33" s="3">
         <v>2</v>
@@ -2576,33 +3413,42 @@
         <v>13</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M33" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C34" s="8">
         <v>3</v>
@@ -2611,33 +3457,42 @@
         <v>#N/A</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="M34" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M34" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="P34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C35" s="6">
         <v>3</v>
@@ -2646,68 +3501,86 @@
         <v>#N/A</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M35" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M35" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P35" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
@@ -2716,24 +3589,33 @@
         <v>13</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P37" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2747,11 +3629,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999E11F1-4A6B-4F19-9DE9-82D2F58C1417}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2850,28 +3732,28 @@
     </row>
     <row r="2" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B2" s="13">
         <v>45541</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="R2">
         <v>20</v>
@@ -2898,39 +3780,39 @@
         <v>400</v>
       </c>
       <c r="Z2">
+        <v>50</v>
+      </c>
+      <c r="AA2">
         <v>20</v>
       </c>
-      <c r="AA2">
-        <v>5</v>
-      </c>
       <c r="AB2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B3" s="13">
         <v>45478</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="P3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="R3">
         <v>20</v>
@@ -2957,39 +3839,39 @@
         <v>400</v>
       </c>
       <c r="Z3">
+        <v>50</v>
+      </c>
+      <c r="AA3">
         <v>20</v>
       </c>
-      <c r="AA3">
-        <v>5</v>
-      </c>
       <c r="AB3">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B4" s="13">
         <v>45541</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="P4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="R4">
         <v>20</v>
@@ -3016,39 +3898,39 @@
         <v>400</v>
       </c>
       <c r="Z4">
+        <v>50</v>
+      </c>
+      <c r="AA4">
         <v>20</v>
       </c>
-      <c r="AA4">
-        <v>5</v>
-      </c>
       <c r="AB4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B5" s="13">
         <v>45541</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="P5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="R5">
         <v>20</v>
@@ -3075,13 +3957,13 @@
         <v>400</v>
       </c>
       <c r="Z5">
+        <v>50</v>
+      </c>
+      <c r="AA5">
         <v>20</v>
       </c>
-      <c r="AA5">
-        <v>5</v>
-      </c>
       <c r="AB5">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>